<commit_message>
Updated publisher jar and reconfigured.
</commit_message>
<xml_diff>
--- a/docs/CareConnect-Flag-1.xlsx
+++ b/docs/CareConnect-Flag-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$39</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="275">
   <si>
     <t>Path</t>
   </si>
@@ -468,7 +468,7 @@
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
   </si>
   <si>
-    <t>http://www.acme.com/identifiers/patient or urn:ietf:rfc:3986 if the Identifier.value itself is a full uri</t>
+    <t>http://www.acme.com/identifiers/patient</t>
   </si>
   <si>
     <t>Identifier.system</t>
@@ -678,79 +678,6 @@
   </si>
   <si>
     <t>The SNOMED CT Description ID for the display.</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.id</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.extension</t>
-  </si>
-  <si>
-    <t>descriptionId</t>
-  </si>
-  <si>
-    <t>The SNOMED CT Description ID</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.extension.id</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.extension.extension</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.extension.url</t>
-  </si>
-  <si>
-    <t>identifies the meaning of the extension</t>
-  </si>
-  <si>
-    <t>Source of the definition for the extension code - a logical name or a URL.</t>
-  </si>
-  <si>
-    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
-  </si>
-  <si>
-    <t>Extension.url</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.extension.valueId</t>
-  </si>
-  <si>
-    <t>valueId</t>
-  </si>
-  <si>
-    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t>descriptionDisplay</t>
-  </si>
-  <si>
-    <t>The SNOMED CT display for the description ID</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.extension.valueString</t>
-  </si>
-  <si>
-    <t>valueString</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.url</t>
-  </si>
-  <si>
-    <t>https://fhir.hl7.org.uk/STU3/StructureDefinition/Extension-coding-sctdescid</t>
-  </si>
-  <si>
-    <t>Flag.code.coding.extension.value[x]</t>
-  </si>
-  <si>
-    <t>base64Binary
-booleancodedatedateTimedecimalidinstantintegermarkdownoidpositiveIntstringtimeunsignedInturiAddressAgeAnnotationAttachmentCodeableConceptCodingContactPointCountDistanceDurationHumanNameIdentifierMoneyPeriodQuantityRangeRatioReferenceSampledDataSignatureTiming</t>
-  </si>
-  <si>
-    <t>Value of extension</t>
   </si>
   <si>
     <t>Flag.code.coding.system</t>
@@ -1089,7 +1016,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK53"/>
+  <dimension ref="A1:AK39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1098,7 +1025,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="45.1484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="28.08984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -4190,7 +4117,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>48</v>
@@ -4202,25 +4129,29 @@
         <v>41</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>111</v>
+        <v>214</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+        <v>215</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>217</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" t="s" s="2">
-        <v>41</v>
+        <v>218</v>
       </c>
       <c r="R30" t="s" s="2">
         <v>41</v>
@@ -4262,7 +4193,7 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>113</v>
+        <v>219</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -4277,7 +4208,7 @@
         <v>41</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>114</v>
+        <v>220</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>41</v>
@@ -4285,7 +4216,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4296,7 +4227,7 @@
         <v>39</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>41</v>
@@ -4305,18 +4236,20 @@
         <v>41</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="M31" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="M31" t="s" s="2">
+        <v>224</v>
+      </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>41</v>
@@ -4353,25 +4286,25 @@
         <v>41</v>
       </c>
       <c r="AA31" t="s" s="2">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="AC31" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD31" t="s" s="2">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>120</v>
+        <v>225</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>41</v>
@@ -4380,7 +4313,7 @@
         <v>41</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>41</v>
+        <v>226</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>41</v>
@@ -4388,11 +4321,9 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="B32" t="s" s="2">
-        <v>215</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
         <v>41</v>
       </c>
@@ -4410,19 +4341,21 @@
         <v>41</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>208</v>
+        <v>229</v>
       </c>
       <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+      <c r="N32" t="s" s="2">
+        <v>230</v>
+      </c>
       <c r="O32" t="s" s="2">
         <v>41</v>
       </c>
@@ -4470,13 +4403,13 @@
         <v>41</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>120</v>
+        <v>231</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>41</v>
@@ -4485,7 +4418,7 @@
         <v>41</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>41</v>
+        <v>232</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>41</v>
@@ -4493,7 +4426,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4501,7 +4434,7 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F33" t="s" s="2">
         <v>48</v>
@@ -4513,19 +4446,21 @@
         <v>41</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J33" t="s" s="2">
         <v>110</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>112</v>
+        <v>235</v>
       </c>
       <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="N33" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="O33" t="s" s="2">
         <v>41</v>
       </c>
@@ -4573,7 +4508,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>113</v>
+        <v>237</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>39</v>
@@ -4588,7 +4523,7 @@
         <v>41</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>114</v>
+        <v>238</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>41</v>
@@ -4596,18 +4531,18 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>41</v>
@@ -4616,21 +4551,23 @@
         <v>41</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>116</v>
+        <v>242</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="N34" s="2"/>
+        <v>243</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>244</v>
+      </c>
       <c r="O34" t="s" s="2">
         <v>41</v>
       </c>
@@ -4666,25 +4603,25 @@
         <v>41</v>
       </c>
       <c r="AA34" t="s" s="2">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="AB34" t="s" s="2">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="AC34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD34" t="s" s="2">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>120</v>
+        <v>245</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>41</v>
@@ -4693,7 +4630,7 @@
         <v>41</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>114</v>
+        <v>246</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>41</v>
@@ -4701,7 +4638,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4709,7 +4646,7 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s" s="2">
         <v>48</v>
@@ -4721,27 +4658,29 @@
         <v>41</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>221</v>
+        <v>249</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>250</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>251</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" t="s" s="2">
-        <v>215</v>
+        <v>41</v>
       </c>
       <c r="R35" t="s" s="2">
         <v>41</v>
@@ -4783,10 +4722,10 @@
         <v>41</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>223</v>
+        <v>252</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>48</v>
@@ -4798,7 +4737,7 @@
         <v>41</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>91</v>
+        <v>253</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>41</v>
@@ -4806,17 +4745,15 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="B36" t="s" s="2">
-        <v>225</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
         <v>41</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>48</v>
@@ -4828,16 +4765,16 @@
         <v>41</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>50</v>
+        <v>255</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>216</v>
+        <v>256</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -4888,10 +4825,10 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>227</v>
+        <v>254</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>48</v>
@@ -4903,25 +4840,23 @@
         <v>41</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>91</v>
+        <v>258</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>41</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="B37" t="s" s="2">
-        <v>228</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
         <v>41</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F37" t="s" s="2">
         <v>48</v>
@@ -4933,16 +4868,16 @@
         <v>41</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>208</v>
+        <v>262</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -4993,13 +4928,13 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>41</v>
@@ -5011,12 +4946,12 @@
         <v>41</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>41</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>217</v>
+        <v>264</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5036,18 +4971,20 @@
         <v>41</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>110</v>
+        <v>265</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>111</v>
+        <v>266</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="M38" s="2"/>
+        <v>267</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>268</v>
+      </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>41</v>
@@ -5096,7 +5033,7 @@
         <v>41</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>113</v>
+        <v>264</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>39</v>
@@ -5111,26 +5048,26 @@
         <v>41</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>41</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>41</v>
@@ -5139,20 +5076,18 @@
         <v>41</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>94</v>
+        <v>270</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>95</v>
+        <v>271</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>97</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>41</v>
@@ -5189,25 +5124,25 @@
         <v>41</v>
       </c>
       <c r="AA39" t="s" s="2">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="AB39" t="s" s="2">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="AC39" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD39" t="s" s="2">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>120</v>
+        <v>269</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>41</v>
@@ -5216,1482 +5151,14 @@
         <v>41</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>114</v>
+        <v>273</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" hidden="true">
-      <c r="A40" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F40" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J40" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P40" s="2"/>
-      <c r="Q40" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="R40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" hidden="true">
-      <c r="A41" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="B41" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="C41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F41" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J41" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="K41" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P41" s="2"/>
-      <c r="Q41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" hidden="true">
-      <c r="A42" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F42" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J42" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="N42" s="2"/>
-      <c r="O42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P42" s="2"/>
-      <c r="Q42" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="R42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE42" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AF42" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" hidden="true">
-      <c r="A43" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J43" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="K43" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P43" s="2"/>
-      <c r="Q43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE43" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI43" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ43" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="AK43" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" hidden="true">
-      <c r="A44" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F44" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I44" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J44" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="K44" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="O44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P44" s="2"/>
-      <c r="Q44" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="R44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="AF44" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG44" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ44" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="AK44" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" hidden="true">
-      <c r="A45" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="B45" s="2"/>
-      <c r="C45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F45" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I45" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J45" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="K45" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N45" s="2"/>
-      <c r="O45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P45" s="2"/>
-      <c r="Q45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE45" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="AF45" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG45" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI45" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ45" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="AK45" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" hidden="true">
-      <c r="A46" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F46" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I46" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J46" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="K46" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="M46" s="2"/>
-      <c r="N46" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="O46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P46" s="2"/>
-      <c r="Q46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE46" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="AF46" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG46" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI46" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ46" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="AK46" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" hidden="true">
-      <c r="A47" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F47" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I47" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J47" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="K47" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="M47" s="2"/>
-      <c r="N47" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="O47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P47" s="2"/>
-      <c r="Q47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="AF47" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG47" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI47" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ47" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="AK47" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" hidden="true">
-      <c r="A48" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F48" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I48" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J48" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="K48" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="O48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P48" s="2"/>
-      <c r="Q48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE48" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AF48" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG48" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI48" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ48" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" hidden="true">
-      <c r="A49" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F49" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I49" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J49" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="K49" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="M49" t="s" s="2">
         <v>274</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="O49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P49" s="2"/>
-      <c r="Q49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE49" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="AF49" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG49" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI49" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ49" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AK49" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" hidden="true">
-      <c r="A50" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F50" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I50" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J50" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P50" s="2"/>
-      <c r="Q50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AG50" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ50" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="51" hidden="true">
-      <c r="A51" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F51" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I51" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J51" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P51" s="2"/>
-      <c r="Q51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="AF51" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG51" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ51" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="52" hidden="true">
-      <c r="A52" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F52" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I52" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J52" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="K52" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="N52" s="2"/>
-      <c r="O52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P52" s="2"/>
-      <c r="Q52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG52" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="53" hidden="true">
-      <c r="A53" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F53" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I53" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J53" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="K53" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P53" s="2"/>
-      <c r="Q53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="AF53" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG53" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>298</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK53">
+  <autoFilter ref="A1:AK39">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6701,7 +5168,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI52">
+  <conditionalFormatting sqref="A2:AI38">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>